<commit_message>
shadow cost of carbon updates
</commit_message>
<xml_diff>
--- a/data/Shadow_Cost_of_Carbon_v10.xlsx
+++ b/data/Shadow_Cost_of_Carbon_v10.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmfernan\dev\repos\standard_inputs\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oburdash\dev\repos\standard_inputs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DD1E46-569E-4CF0-A1E3-8491E0FB4F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553EB033-6F10-4D51-ADEB-AAF13874BE7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="12780" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="4" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="95">
   <si>
     <t>Project |</t>
   </si>
@@ -340,40 +340,6 @@
   <si>
     <t>Carbon cost</t>
   </si>
-  <si>
-    <r>
-      <t>EU27 €</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <rFont val="Roboto"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2016</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Roboto"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/tCO2</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <rFont val="Roboto"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>eq</t>
-    </r>
-  </si>
 </sst>
 </file>
 
@@ -385,7 +351,7 @@
     <numFmt numFmtId="165" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -456,21 +422,8 @@
       <color theme="9"/>
       <name val="Roboto"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Roboto"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <vertAlign val="subscript"/>
-      <sz val="11"/>
-      <name val="Roboto"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -522,12 +475,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -623,7 +570,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -760,13 +707,11 @@
     <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -789,9 +734,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF103E69"/>
       <color rgb="FF2990EA"/>
       <color rgb="FF003366"/>
-      <color rgb="FF103E69"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1544,6 +1489,524 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.7347933635692635E-2"/>
+          <c:y val="2.5583428638163246E-2"/>
+          <c:w val="0.89264410656177584"/>
+          <c:h val="0.83015153730986835"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tidy_Data!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cost</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="&quot;€&quot;#,##0" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="103E69"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tidy_Data!$A$2:$A$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2032</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2033</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2034</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2036</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2037</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2038</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2039</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2041</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2042</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2043</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2044</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2045</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2046</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2047</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2049</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tidy_Data!$B$2:$B$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>105.365741665003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>123.831902575364</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>142.298063485726</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>160.764224396087</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>179.230385306448</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>197.69654621680999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>216.16270712717099</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>234.62886803753199</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>253.09502894789401</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>271.56118985825498</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>301.97604312238002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>332.39089638650398</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>362.80574965062902</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>393.22060291475299</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>423.63545617887797</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>452.96406468356997</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>482.29267318826101</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>511.621281692953</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>540.94989019764398</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>570.27849870233604</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>599.60710720702696</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>628.93571571171901</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>658.26432421641005</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>687.59293272110199</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>716.92154122579302</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>747.33639448991801</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>777.75124775404299</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>808.16610101816696</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>838.58095428229205</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>868.99580754641602</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9CC6-4402-9D47-0964CD8D6585}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="20"/>
+        <c:overlap val="-27"/>
+        <c:axId val="271805360"/>
+        <c:axId val="417483104"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="271805360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-2700000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="103E69"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="417483104"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="417483104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="103E69"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1800" b="1"/>
+                  <a:t>Cost of carbon</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="103E69"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="&quot;€&quot;#,##0.00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="103E69"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="271805360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400">
+          <a:solidFill>
+            <a:srgbClr val="103E69"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2510,6 +2973,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
@@ -3016,6 +3519,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3771,6 +4777,47 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>461960</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A2AA00D-F75F-646A-DF00-06D56599D8EB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5087,336 +6134,336 @@
       <c r="Q2" s="2"/>
     </row>
     <row r="3" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="N3" s="59" t="s">
+      <c r="N3" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="59"/>
+      <c r="O3" s="57"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
     </row>
     <row r="4" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="N4" s="59"/>
-      <c r="O4" s="59"/>
+      <c r="N4" s="57"/>
+      <c r="O4" s="57"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
     </row>
     <row r="5" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="N5" s="59"/>
-      <c r="O5" s="59"/>
+      <c r="N5" s="57"/>
+      <c r="O5" s="57"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
     </row>
     <row r="6" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="N6" s="59"/>
-      <c r="O6" s="59"/>
+      <c r="N6" s="57"/>
+      <c r="O6" s="57"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
     </row>
     <row r="7" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="N7" s="59"/>
-      <c r="O7" s="59"/>
+      <c r="N7" s="57"/>
+      <c r="O7" s="57"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
     </row>
     <row r="8" spans="2:17" s="11" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="60"/>
-      <c r="L8" s="60"/>
-      <c r="M8" s="60"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="58"/>
+      <c r="K8" s="58"/>
+      <c r="L8" s="58"/>
+      <c r="M8" s="58"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
     </row>
     <row r="9" spans="2:17" s="11" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="60"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="60"/>
-      <c r="L9" s="60"/>
-      <c r="M9" s="60"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="58"/>
+      <c r="M9" s="58"/>
     </row>
     <row r="10" spans="2:17" s="11" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="60"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="60"/>
-      <c r="L10" s="60"/>
-      <c r="M10" s="60"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="58"/>
     </row>
     <row r="11" spans="2:17" s="11" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="60"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="60"/>
-      <c r="K11" s="60"/>
-      <c r="L11" s="60"/>
-      <c r="M11" s="60"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="58"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="58"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="58"/>
+      <c r="M11" s="58"/>
     </row>
     <row r="12" spans="2:17" s="11" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="60"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="60"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="60"/>
-      <c r="L12" s="60"/>
-      <c r="M12" s="60"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="58"/>
+      <c r="H12" s="58"/>
+      <c r="I12" s="58"/>
+      <c r="J12" s="58"/>
+      <c r="K12" s="58"/>
+      <c r="L12" s="58"/>
+      <c r="M12" s="58"/>
     </row>
     <row r="13" spans="2:17" s="11" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="60"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="60"/>
-      <c r="L13" s="60"/>
-      <c r="M13" s="60"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="58"/>
+      <c r="K13" s="58"/>
+      <c r="L13" s="58"/>
+      <c r="M13" s="58"/>
     </row>
     <row r="14" spans="2:17" s="11" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="60"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="60"/>
-      <c r="L14" s="60"/>
-      <c r="M14" s="60"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="58"/>
+      <c r="L14" s="58"/>
+      <c r="M14" s="58"/>
     </row>
     <row r="15" spans="2:17" s="11" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="60"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="60"/>
-      <c r="G15" s="60"/>
-      <c r="H15" s="60"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="60"/>
-      <c r="K15" s="60"/>
-      <c r="L15" s="60"/>
-      <c r="M15" s="60"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="58"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="58"/>
+      <c r="G15" s="58"/>
+      <c r="H15" s="58"/>
+      <c r="I15" s="58"/>
+      <c r="J15" s="58"/>
+      <c r="K15" s="58"/>
+      <c r="L15" s="58"/>
+      <c r="M15" s="58"/>
     </row>
     <row r="16" spans="2:17" s="11" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="60"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="60"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="60"/>
-      <c r="J16" s="60"/>
-      <c r="K16" s="60"/>
-      <c r="L16" s="60"/>
-      <c r="M16" s="60"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="58"/>
+      <c r="K16" s="58"/>
+      <c r="L16" s="58"/>
+      <c r="M16" s="58"/>
     </row>
     <row r="17" spans="2:13" s="11" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="60"/>
-      <c r="C17" s="60"/>
-      <c r="D17" s="60"/>
-      <c r="E17" s="60"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="60"/>
-      <c r="H17" s="60"/>
-      <c r="I17" s="60"/>
-      <c r="J17" s="60"/>
-      <c r="K17" s="60"/>
-      <c r="L17" s="60"/>
-      <c r="M17" s="60"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="58"/>
+      <c r="L17" s="58"/>
+      <c r="M17" s="58"/>
     </row>
     <row r="18" spans="2:13" s="11" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="60"/>
-      <c r="C18" s="60"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="60"/>
-      <c r="G18" s="60"/>
-      <c r="H18" s="60"/>
-      <c r="I18" s="60"/>
-      <c r="J18" s="60"/>
-      <c r="K18" s="60"/>
-      <c r="L18" s="60"/>
-      <c r="M18" s="60"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="58"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="58"/>
+      <c r="G18" s="58"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="58"/>
+      <c r="K18" s="58"/>
+      <c r="L18" s="58"/>
+      <c r="M18" s="58"/>
     </row>
     <row r="19" spans="2:13" s="11" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="60"/>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="60"/>
-      <c r="H19" s="60"/>
-      <c r="I19" s="60"/>
-      <c r="J19" s="60"/>
-      <c r="K19" s="60"/>
-      <c r="L19" s="60"/>
-      <c r="M19" s="60"/>
+      <c r="B19" s="58"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="58"/>
+      <c r="K19" s="58"/>
+      <c r="L19" s="58"/>
+      <c r="M19" s="58"/>
     </row>
     <row r="20" spans="2:13" s="11" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="61" t="s">
+      <c r="B20" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="61"/>
-      <c r="D20" s="61"/>
-      <c r="E20" s="61"/>
-      <c r="F20" s="61"/>
-      <c r="G20" s="61"/>
-      <c r="H20" s="61"/>
-      <c r="I20" s="61"/>
-      <c r="J20" s="61"/>
-      <c r="K20" s="61"/>
-      <c r="L20" s="61"/>
-      <c r="M20" s="61"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="59"/>
+      <c r="H20" s="59"/>
+      <c r="I20" s="59"/>
+      <c r="J20" s="59"/>
+      <c r="K20" s="59"/>
+      <c r="L20" s="59"/>
+      <c r="M20" s="59"/>
     </row>
     <row r="21" spans="2:13" s="11" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="61"/>
-      <c r="C21" s="61"/>
-      <c r="D21" s="61"/>
-      <c r="E21" s="61"/>
-      <c r="F21" s="61"/>
-      <c r="G21" s="61"/>
-      <c r="H21" s="61"/>
-      <c r="I21" s="61"/>
-      <c r="J21" s="61"/>
-      <c r="K21" s="61"/>
-      <c r="L21" s="61"/>
-      <c r="M21" s="61"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="59"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="59"/>
+      <c r="J21" s="59"/>
+      <c r="K21" s="59"/>
+      <c r="L21" s="59"/>
+      <c r="M21" s="59"/>
     </row>
     <row r="22" spans="2:13" s="11" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="61"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="61"/>
-      <c r="E22" s="61"/>
-      <c r="F22" s="61"/>
-      <c r="G22" s="61"/>
-      <c r="H22" s="61"/>
-      <c r="I22" s="61"/>
-      <c r="J22" s="61"/>
-      <c r="K22" s="61"/>
-      <c r="L22" s="61"/>
-      <c r="M22" s="61"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="59"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="59"/>
+      <c r="J22" s="59"/>
+      <c r="K22" s="59"/>
+      <c r="L22" s="59"/>
+      <c r="M22" s="59"/>
     </row>
     <row r="23" spans="2:13" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="62"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="62"/>
-      <c r="L23" s="62"/>
-      <c r="M23" s="62"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="60"/>
+      <c r="I23" s="60"/>
+      <c r="J23" s="60"/>
+      <c r="K23" s="60"/>
+      <c r="L23" s="60"/>
+      <c r="M23" s="60"/>
     </row>
     <row r="24" spans="2:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="62"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="62"/>
-      <c r="G24" s="62"/>
-      <c r="H24" s="62"/>
-      <c r="I24" s="62"/>
-      <c r="J24" s="62"/>
-      <c r="K24" s="62"/>
-      <c r="L24" s="62"/>
-      <c r="M24" s="62"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="60"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="60"/>
+      <c r="H24" s="60"/>
+      <c r="I24" s="60"/>
+      <c r="J24" s="60"/>
+      <c r="K24" s="60"/>
+      <c r="L24" s="60"/>
+      <c r="M24" s="60"/>
     </row>
     <row r="25" spans="2:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="62"/>
-      <c r="C25" s="62"/>
-      <c r="D25" s="62"/>
-      <c r="E25" s="62"/>
-      <c r="F25" s="62"/>
-      <c r="G25" s="62"/>
-      <c r="H25" s="62"/>
-      <c r="I25" s="62"/>
-      <c r="J25" s="62"/>
-      <c r="K25" s="62"/>
-      <c r="L25" s="62"/>
-      <c r="M25" s="62"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="60"/>
+      <c r="I25" s="60"/>
+      <c r="J25" s="60"/>
+      <c r="K25" s="60"/>
+      <c r="L25" s="60"/>
+      <c r="M25" s="60"/>
     </row>
     <row r="26" spans="2:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="62"/>
-      <c r="C26" s="62"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="62"/>
-      <c r="G26" s="62"/>
-      <c r="H26" s="62"/>
-      <c r="I26" s="62"/>
-      <c r="J26" s="62"/>
-      <c r="K26" s="62"/>
-      <c r="L26" s="62"/>
-      <c r="M26" s="62"/>
+      <c r="B26" s="60"/>
+      <c r="C26" s="60"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="60"/>
+      <c r="F26" s="60"/>
+      <c r="G26" s="60"/>
+      <c r="H26" s="60"/>
+      <c r="I26" s="60"/>
+      <c r="J26" s="60"/>
+      <c r="K26" s="60"/>
+      <c r="L26" s="60"/>
+      <c r="M26" s="60"/>
     </row>
     <row r="27" spans="2:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="62"/>
-      <c r="C27" s="62"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="62"/>
-      <c r="F27" s="62"/>
-      <c r="G27" s="62"/>
-      <c r="H27" s="62"/>
-      <c r="I27" s="62"/>
-      <c r="J27" s="62"/>
-      <c r="K27" s="62"/>
-      <c r="L27" s="62"/>
-      <c r="M27" s="62"/>
+      <c r="B27" s="60"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="60"/>
+      <c r="I27" s="60"/>
+      <c r="J27" s="60"/>
+      <c r="K27" s="60"/>
+      <c r="L27" s="60"/>
+      <c r="M27" s="60"/>
     </row>
     <row r="28" spans="2:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="62"/>
-      <c r="C28" s="62"/>
-      <c r="D28" s="62"/>
-      <c r="E28" s="62"/>
-      <c r="F28" s="62"/>
-      <c r="G28" s="62"/>
-      <c r="H28" s="62"/>
-      <c r="I28" s="62"/>
-      <c r="J28" s="62"/>
-      <c r="K28" s="62"/>
-      <c r="L28" s="62"/>
-      <c r="M28" s="62"/>
+      <c r="B28" s="60"/>
+      <c r="C28" s="60"/>
+      <c r="D28" s="60"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="60"/>
+      <c r="H28" s="60"/>
+      <c r="I28" s="60"/>
+      <c r="J28" s="60"/>
+      <c r="K28" s="60"/>
+      <c r="L28" s="60"/>
+      <c r="M28" s="60"/>
     </row>
     <row r="29" spans="2:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="12" t="s">
@@ -14805,10 +15852,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B46B1E9-73C3-45B5-8A8A-E84DD80BDC08}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14817,259 +15864,257 @@
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="58" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="54">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>2021</v>
       </c>
-      <c r="B2" s="55">
+      <c r="B2">
         <v>105.365741665003</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="54">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2022</v>
       </c>
-      <c r="B3" s="55">
+      <c r="B3">
         <v>123.831902575364</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="54">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>2023</v>
       </c>
-      <c r="B4" s="55">
+      <c r="B4">
         <v>142.298063485726</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="54">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>2024</v>
       </c>
-      <c r="B5" s="55">
+      <c r="B5">
         <v>160.764224396087</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="54">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>2025</v>
       </c>
-      <c r="B6" s="55">
+      <c r="B6">
         <v>179.230385306448</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="54">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>2026</v>
       </c>
-      <c r="B7" s="55">
+      <c r="B7">
         <v>197.69654621680999</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="54">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>2027</v>
       </c>
-      <c r="B8" s="55">
+      <c r="B8">
         <v>216.16270712717099</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="54">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>2028</v>
       </c>
-      <c r="B9" s="55">
+      <c r="B9">
         <v>234.62886803753199</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="54">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>2029</v>
       </c>
-      <c r="B10" s="55">
+      <c r="B10">
         <v>253.09502894789401</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="54">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>2030</v>
       </c>
-      <c r="B11" s="55">
+      <c r="B11">
         <v>271.56118985825498</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="54">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>2031</v>
       </c>
-      <c r="B12" s="55">
+      <c r="B12">
         <v>301.97604312238002</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="54">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>2032</v>
       </c>
-      <c r="B13" s="55">
+      <c r="B13">
         <v>332.39089638650398</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="54">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>2033</v>
       </c>
-      <c r="B14" s="55">
+      <c r="B14">
         <v>362.80574965062902</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="54">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>2034</v>
       </c>
-      <c r="B15" s="55">
+      <c r="B15">
         <v>393.22060291475299</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="54">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>2035</v>
       </c>
-      <c r="B16" s="55">
+      <c r="B16">
         <v>423.63545617887797</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="54">
+      <c r="A17">
         <v>2036</v>
       </c>
-      <c r="B17" s="55">
+      <c r="B17">
         <v>452.96406468356997</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="54">
+      <c r="A18">
         <v>2037</v>
       </c>
-      <c r="B18" s="55">
+      <c r="B18">
         <v>482.29267318826101</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="54">
+      <c r="A19">
         <v>2038</v>
       </c>
-      <c r="B19" s="55">
+      <c r="B19">
         <v>511.621281692953</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="54">
+      <c r="A20">
         <v>2039</v>
       </c>
-      <c r="B20" s="55">
+      <c r="B20">
         <v>540.94989019764398</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="54">
+      <c r="A21">
         <v>2040</v>
       </c>
-      <c r="B21" s="55">
+      <c r="B21">
         <v>570.27849870233604</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="54">
+      <c r="A22">
         <v>2041</v>
       </c>
-      <c r="B22" s="55">
+      <c r="B22">
         <v>599.60710720702696</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="54">
+      <c r="A23">
         <v>2042</v>
       </c>
-      <c r="B23" s="55">
+      <c r="B23">
         <v>628.93571571171901</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="54">
+      <c r="A24">
         <v>2043</v>
       </c>
-      <c r="B24" s="55">
+      <c r="B24">
         <v>658.26432421641005</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="54">
+      <c r="A25">
         <v>2044</v>
       </c>
-      <c r="B25" s="55">
+      <c r="B25">
         <v>687.59293272110199</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="54">
+      <c r="A26">
         <v>2045</v>
       </c>
-      <c r="B26" s="55">
+      <c r="B26">
         <v>716.92154122579302</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="54">
+      <c r="A27">
         <v>2046</v>
       </c>
-      <c r="B27" s="55">
+      <c r="B27">
         <v>747.33639448991801</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="54">
+      <c r="A28">
         <v>2047</v>
       </c>
-      <c r="B28" s="55">
+      <c r="B28">
         <v>777.75124775404299</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="54">
+      <c r="A29">
         <v>2048</v>
       </c>
-      <c r="B29" s="55">
+      <c r="B29">
         <v>808.16610101816696</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="54">
+      <c r="A30">
         <v>2049</v>
       </c>
-      <c r="B30" s="55">
+      <c r="B30">
         <v>838.58095428229205</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="54">
+      <c r="A31">
         <v>2050</v>
       </c>
-      <c r="B31" s="55">
+      <c r="B31">
         <v>868.99580754641602</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -15088,7 +16133,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="55" t="s">
         <v>92</v>
       </c>
       <c r="B2" t="s">
@@ -15096,250 +16141,250 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="57">
+      <c r="A3" s="56">
         <v>2021</v>
       </c>
-      <c r="B3" s="55">
+      <c r="B3" s="54">
         <v>105.365741665003</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="57">
+      <c r="A4" s="56">
         <v>2022</v>
       </c>
-      <c r="B4" s="55">
+      <c r="B4" s="54">
         <v>123.831902575364</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="57">
+      <c r="A5" s="56">
         <v>2023</v>
       </c>
-      <c r="B5" s="55">
+      <c r="B5" s="54">
         <v>142.298063485726</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="57">
+      <c r="A6" s="56">
         <v>2024</v>
       </c>
-      <c r="B6" s="55">
+      <c r="B6" s="54">
         <v>160.764224396087</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="57">
+      <c r="A7" s="56">
         <v>2025</v>
       </c>
-      <c r="B7" s="55">
+      <c r="B7" s="54">
         <v>179.230385306448</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="57">
+      <c r="A8" s="56">
         <v>2026</v>
       </c>
-      <c r="B8" s="55">
+      <c r="B8" s="54">
         <v>197.69654621680999</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="57">
+      <c r="A9" s="56">
         <v>2027</v>
       </c>
-      <c r="B9" s="55">
+      <c r="B9" s="54">
         <v>216.16270712717099</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="57">
+      <c r="A10" s="56">
         <v>2028</v>
       </c>
-      <c r="B10" s="55">
+      <c r="B10" s="54">
         <v>234.62886803753199</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="57">
+      <c r="A11" s="56">
         <v>2029</v>
       </c>
-      <c r="B11" s="55">
+      <c r="B11" s="54">
         <v>253.09502894789401</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="57">
+      <c r="A12" s="56">
         <v>2030</v>
       </c>
-      <c r="B12" s="55">
+      <c r="B12" s="54">
         <v>271.56118985825498</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="57">
+      <c r="A13" s="56">
         <v>2031</v>
       </c>
-      <c r="B13" s="55">
+      <c r="B13" s="54">
         <v>301.97604312238002</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="57">
+      <c r="A14" s="56">
         <v>2032</v>
       </c>
-      <c r="B14" s="55">
+      <c r="B14" s="54">
         <v>332.39089638650398</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="57">
+      <c r="A15" s="56">
         <v>2033</v>
       </c>
-      <c r="B15" s="55">
+      <c r="B15" s="54">
         <v>362.80574965062902</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="57">
+      <c r="A16" s="56">
         <v>2034</v>
       </c>
-      <c r="B16" s="55">
+      <c r="B16" s="54">
         <v>393.22060291475299</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="57">
+      <c r="A17" s="56">
         <v>2035</v>
       </c>
-      <c r="B17" s="55">
+      <c r="B17" s="54">
         <v>423.63545617887797</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="57">
+      <c r="A18" s="56">
         <v>2036</v>
       </c>
-      <c r="B18" s="55">
+      <c r="B18" s="54">
         <v>452.96406468356997</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="57">
+      <c r="A19" s="56">
         <v>2037</v>
       </c>
-      <c r="B19" s="55">
+      <c r="B19" s="54">
         <v>482.29267318826101</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="57">
+      <c r="A20" s="56">
         <v>2038</v>
       </c>
-      <c r="B20" s="55">
+      <c r="B20" s="54">
         <v>511.621281692953</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="57">
+      <c r="A21" s="56">
         <v>2039</v>
       </c>
-      <c r="B21" s="55">
+      <c r="B21" s="54">
         <v>540.94989019764398</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="57">
+      <c r="A22" s="56">
         <v>2040</v>
       </c>
-      <c r="B22" s="55">
+      <c r="B22" s="54">
         <v>570.27849870233604</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="57">
+      <c r="A23" s="56">
         <v>2041</v>
       </c>
-      <c r="B23" s="55">
+      <c r="B23" s="54">
         <v>599.60710720702696</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="57">
+      <c r="A24" s="56">
         <v>2042</v>
       </c>
-      <c r="B24" s="55">
+      <c r="B24" s="54">
         <v>628.93571571171901</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="57">
+      <c r="A25" s="56">
         <v>2043</v>
       </c>
-      <c r="B25" s="55">
+      <c r="B25" s="54">
         <v>658.26432421641005</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="57">
+      <c r="A26" s="56">
         <v>2044</v>
       </c>
-      <c r="B26" s="55">
+      <c r="B26" s="54">
         <v>687.59293272110199</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="57">
+      <c r="A27" s="56">
         <v>2045</v>
       </c>
-      <c r="B27" s="55">
+      <c r="B27" s="54">
         <v>716.92154122579302</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="57">
+      <c r="A28" s="56">
         <v>2046</v>
       </c>
-      <c r="B28" s="55">
+      <c r="B28" s="54">
         <v>747.33639448991801</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="57">
+      <c r="A29" s="56">
         <v>2047</v>
       </c>
-      <c r="B29" s="55">
+      <c r="B29" s="54">
         <v>777.75124775404299</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="57">
+      <c r="A30" s="56">
         <v>2048</v>
       </c>
-      <c r="B30" s="55">
+      <c r="B30" s="54">
         <v>808.16610101816696</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="57">
+      <c r="A31" s="56">
         <v>2049</v>
       </c>
-      <c r="B31" s="55">
+      <c r="B31" s="54">
         <v>838.58095428229205</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="57">
+      <c r="A32" s="56">
         <v>2050</v>
       </c>
-      <c r="B32" s="55">
+      <c r="B32" s="54">
         <v>868.99580754641602</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="57" t="s">
+      <c r="A33" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="B33" s="55">
+      <c r="B33" s="54">
         <v>13588.921940507083</v>
       </c>
     </row>
@@ -18544,12 +19589,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100763DCA751E988E49B18D7A5F3E2E0A59" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7de07ceb4021a46e644f2475dce3c08e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="841a37d2-6ac6-4cb8-8211-c8824e7b4dcd" xmlns:ns3="c78a888a-83d8-49bb-8890-6eb97e8a3c0e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a575a7fa9043b0502b32047f1ff6be7" ns2:_="" ns3:_="">
     <xsd:import namespace="841a37d2-6ac6-4cb8-8211-c8824e7b4dcd"/>
@@ -18772,6 +19811,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{725F688E-8702-4916-9D48-F0F82F4E0F2E}">
   <ds:schemaRefs>
@@ -18781,23 +19826,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A93D3A15-F8BB-44A4-BB5B-995A4B735684}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="c78a888a-83d8-49bb-8890-6eb97e8a3c0e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="841a37d2-6ac6-4cb8-8211-c8824e7b4dcd"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C1F8D52-AAD7-42F8-89D3-E5D0A58CB3FC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18814,4 +19842,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A93D3A15-F8BB-44A4-BB5B-995A4B735684}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="c78a888a-83d8-49bb-8890-6eb97e8a3c0e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="841a37d2-6ac6-4cb8-8211-c8824e7b4dcd"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>